<commit_message>
fix: Apr 24 update
</commit_message>
<xml_diff>
--- a/data/Texas COVID-19 Case Count Data by County.xlsx
+++ b/data/Texas COVID-19 Case Count Data by County.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\CHS-AAU\Epi\Covid\For Ektron\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{22A52665-D8B6-4598-9D36-4758E4DE69B7}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{E61C2237-8237-42D3-B726-62F926F18C21}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8730" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="314">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="315">
   <si>
     <t>Population</t>
   </si>
@@ -1052,7 +1052,11 @@
 04-22</t>
   </si>
   <si>
-    <t>COVID-19 Total Cases by County, March 4 - April 22*</t>
+    <t>Cases 
+04-23</t>
+  </si>
+  <si>
+    <t>COVID-19 Total Cases by County, March 4 - April 23*</t>
   </si>
 </sst>
 </file>
@@ -1804,7 +1808,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AW401"/>
+  <dimension ref="A1:AX401"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -1825,11 +1829,11 @@
     <col min="34" max="34" width="10.81640625" style="11" customWidth="1"/>
     <col min="35" max="35" width="9.7265625" style="11" bestFit="1" customWidth="1"/>
     <col min="36" max="43" width="11" style="11" bestFit="1" customWidth="1"/>
-    <col min="44" max="49" width="11" style="53" bestFit="1" customWidth="1"/>
-    <col min="50" max="16384" width="8.7265625" style="11"/>
+    <col min="44" max="50" width="11" style="53" bestFit="1" customWidth="1"/>
+    <col min="51" max="16384" width="8.7265625" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:49" s="22" customFormat="1" ht="67.900000000000006" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:50" s="22" customFormat="1" ht="67.900000000000006" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="19"/>
       <c r="B1" s="20"/>
       <c r="C1" s="20"/>
@@ -1842,7 +1846,7 @@
       <c r="J1" s="20"/>
       <c r="K1" s="20"/>
       <c r="L1" s="21" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="M1" s="20"/>
       <c r="N1" s="20"/>
@@ -1868,8 +1872,9 @@
       <c r="AU1" s="48"/>
       <c r="AV1" s="48"/>
       <c r="AW1" s="48"/>
+      <c r="AX1" s="48"/>
     </row>
-    <row r="2" spans="1:49" s="22" customFormat="1" ht="41.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:50" s="22" customFormat="1" ht="41.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="58" t="s">
         <v>297</v>
       </c>
@@ -1907,8 +1912,9 @@
       <c r="AU2" s="48"/>
       <c r="AV2" s="48"/>
       <c r="AW2" s="48"/>
+      <c r="AX2" s="48"/>
     </row>
-    <row r="3" spans="1:49" s="12" customFormat="1" ht="44.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:50" s="12" customFormat="1" ht="44.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="24" t="s">
         <v>259</v>
       </c>
@@ -2056,8 +2062,11 @@
       <c r="AW3" s="49" t="s">
         <v>312</v>
       </c>
+      <c r="AX3" s="49" t="s">
+        <v>313</v>
+      </c>
     </row>
-    <row r="4" spans="1:49" s="12" customFormat="1" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:50" s="12" customFormat="1" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="26" t="s">
         <v>2</v>
       </c>
@@ -2205,8 +2214,11 @@
       <c r="AW4" s="50">
         <v>14</v>
       </c>
+      <c r="AX4" s="50">
+        <v>14</v>
+      </c>
     </row>
-    <row r="5" spans="1:49" s="27" customFormat="1" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:50" s="27" customFormat="1" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="26" t="s">
         <v>3</v>
       </c>
@@ -2354,8 +2366,11 @@
       <c r="AW5" s="50">
         <v>19</v>
       </c>
+      <c r="AX5" s="50">
+        <v>19</v>
+      </c>
     </row>
-    <row r="6" spans="1:49" s="27" customFormat="1" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:50" s="27" customFormat="1" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="26" t="s">
         <v>4</v>
       </c>
@@ -2503,8 +2518,11 @@
       <c r="AW6" s="50">
         <v>30</v>
       </c>
+      <c r="AX6" s="50">
+        <v>31</v>
+      </c>
     </row>
-    <row r="7" spans="1:49" s="27" customFormat="1" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:50" s="27" customFormat="1" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="26" t="s">
         <v>5</v>
       </c>
@@ -2652,8 +2670,11 @@
       <c r="AW7" s="50">
         <v>2</v>
       </c>
+      <c r="AX7" s="50">
+        <v>2</v>
+      </c>
     </row>
-    <row r="8" spans="1:49" s="12" customFormat="1" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:50" s="12" customFormat="1" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="26" t="s">
         <v>6</v>
       </c>
@@ -2801,8 +2822,11 @@
       <c r="AW8" s="50">
         <v>0</v>
       </c>
+      <c r="AX8" s="50">
+        <v>0</v>
+      </c>
     </row>
-    <row r="9" spans="1:49" s="12" customFormat="1" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:50" s="12" customFormat="1" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="26" t="s">
         <v>7</v>
       </c>
@@ -2950,8 +2974,11 @@
       <c r="AW9" s="50">
         <v>1</v>
       </c>
+      <c r="AX9" s="50">
+        <v>1</v>
+      </c>
     </row>
-    <row r="10" spans="1:49" s="12" customFormat="1" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:50" s="12" customFormat="1" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="26" t="s">
         <v>8</v>
       </c>
@@ -3099,8 +3126,11 @@
       <c r="AW10" s="50">
         <v>14</v>
       </c>
+      <c r="AX10" s="50">
+        <v>14</v>
+      </c>
     </row>
-    <row r="11" spans="1:49" s="12" customFormat="1" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:50" s="12" customFormat="1" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="26" t="s">
         <v>9</v>
       </c>
@@ -3248,8 +3278,11 @@
       <c r="AW11" s="50">
         <v>12</v>
       </c>
+      <c r="AX11" s="50">
+        <v>12</v>
+      </c>
     </row>
-    <row r="12" spans="1:49" s="12" customFormat="1" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:50" s="12" customFormat="1" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="26" t="s">
         <v>10</v>
       </c>
@@ -3397,8 +3430,11 @@
       <c r="AW12" s="50">
         <v>0</v>
       </c>
+      <c r="AX12" s="50">
+        <v>0</v>
+      </c>
     </row>
-    <row r="13" spans="1:49" s="12" customFormat="1" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:50" s="12" customFormat="1" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="26" t="s">
         <v>11</v>
       </c>
@@ -3546,8 +3582,11 @@
       <c r="AW13" s="50">
         <v>4</v>
       </c>
+      <c r="AX13" s="50">
+        <v>4</v>
+      </c>
     </row>
-    <row r="14" spans="1:49" s="27" customFormat="1" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:50" s="27" customFormat="1" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="26" t="s">
         <v>12</v>
       </c>
@@ -3695,8 +3734,11 @@
       <c r="AW14" s="50">
         <v>51</v>
       </c>
+      <c r="AX14" s="50">
+        <v>53</v>
+      </c>
     </row>
-    <row r="15" spans="1:49" s="27" customFormat="1" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:50" s="27" customFormat="1" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="26" t="s">
         <v>13</v>
       </c>
@@ -3844,8 +3886,11 @@
       <c r="AW15" s="50">
         <v>0</v>
       </c>
+      <c r="AX15" s="50">
+        <v>0</v>
+      </c>
     </row>
-    <row r="16" spans="1:49" s="12" customFormat="1" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:50" s="12" customFormat="1" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="26" t="s">
         <v>14</v>
       </c>
@@ -3993,8 +4038,11 @@
       <c r="AW16" s="50">
         <v>5</v>
       </c>
+      <c r="AX16" s="50">
+        <v>6</v>
+      </c>
     </row>
-    <row r="17" spans="1:49" s="12" customFormat="1" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:50" s="12" customFormat="1" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="26" t="s">
         <v>15</v>
       </c>
@@ -4142,8 +4190,11 @@
       <c r="AW17" s="50">
         <v>145</v>
       </c>
+      <c r="AX17" s="50">
+        <v>153</v>
+      </c>
     </row>
-    <row r="18" spans="1:49" s="12" customFormat="1" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:50" s="12" customFormat="1" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="26" t="s">
         <v>16</v>
       </c>
@@ -4291,8 +4342,11 @@
       <c r="AW18" s="50">
         <v>1080</v>
       </c>
+      <c r="AX18" s="50">
+        <v>1126</v>
+      </c>
     </row>
-    <row r="19" spans="1:49" s="12" customFormat="1" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:50" s="12" customFormat="1" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="26" t="s">
         <v>17</v>
       </c>
@@ -4440,8 +4494,11 @@
       <c r="AW19" s="50">
         <v>5</v>
       </c>
+      <c r="AX19" s="50">
+        <v>6</v>
+      </c>
     </row>
-    <row r="20" spans="1:49" s="12" customFormat="1" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:50" s="12" customFormat="1" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="26" t="s">
         <v>18</v>
       </c>
@@ -4589,8 +4646,11 @@
       <c r="AW20" s="50">
         <v>0</v>
       </c>
+      <c r="AX20" s="50">
+        <v>0</v>
+      </c>
     </row>
-    <row r="21" spans="1:49" s="12" customFormat="1" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:50" s="12" customFormat="1" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="26" t="s">
         <v>19</v>
       </c>
@@ -4738,8 +4798,11 @@
       <c r="AW21" s="50">
         <v>3</v>
       </c>
+      <c r="AX21" s="50">
+        <v>3</v>
+      </c>
     </row>
-    <row r="22" spans="1:49" s="12" customFormat="1" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:50" s="12" customFormat="1" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="26" t="s">
         <v>20</v>
       </c>
@@ -4887,8 +4950,11 @@
       <c r="AW22" s="50">
         <v>66</v>
       </c>
+      <c r="AX22" s="50">
+        <v>66</v>
+      </c>
     </row>
-    <row r="23" spans="1:49" s="27" customFormat="1" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:50" s="27" customFormat="1" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="26" t="s">
         <v>21</v>
       </c>
@@ -5036,8 +5102,11 @@
       <c r="AW23" s="50">
         <v>345</v>
       </c>
+      <c r="AX23" s="50">
+        <v>382</v>
+      </c>
     </row>
-    <row r="24" spans="1:49" s="12" customFormat="1" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:50" s="12" customFormat="1" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="26" t="s">
         <v>22</v>
       </c>
@@ -5185,8 +5254,11 @@
       <c r="AW24" s="50">
         <v>173</v>
       </c>
+      <c r="AX24" s="50">
+        <v>177</v>
+      </c>
     </row>
-    <row r="25" spans="1:49" s="12" customFormat="1" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:50" s="12" customFormat="1" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="26" t="s">
         <v>23</v>
       </c>
@@ -5334,8 +5406,11 @@
       <c r="AW25" s="50">
         <v>0</v>
       </c>
+      <c r="AX25" s="50">
+        <v>0</v>
+      </c>
     </row>
-    <row r="26" spans="1:49" s="12" customFormat="1" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:50" s="12" customFormat="1" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="26" t="s">
         <v>24</v>
       </c>
@@ -5483,8 +5558,11 @@
       <c r="AW26" s="50">
         <v>0</v>
       </c>
+      <c r="AX26" s="50">
+        <v>0</v>
+      </c>
     </row>
-    <row r="27" spans="1:49" s="12" customFormat="1" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:50" s="12" customFormat="1" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="26" t="s">
         <v>25</v>
       </c>
@@ -5632,8 +5710,11 @@
       <c r="AW27" s="50">
         <v>1</v>
       </c>
+      <c r="AX27" s="50">
+        <v>1</v>
+      </c>
     </row>
-    <row r="28" spans="1:49" s="27" customFormat="1" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:50" s="27" customFormat="1" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="26" t="s">
         <v>26</v>
       </c>
@@ -5781,8 +5862,11 @@
       <c r="AW28" s="50">
         <v>13</v>
       </c>
+      <c r="AX28" s="50">
+        <v>13</v>
+      </c>
     </row>
-    <row r="29" spans="1:49" s="12" customFormat="1" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:50" s="12" customFormat="1" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="26" t="s">
         <v>27</v>
       </c>
@@ -5930,8 +6014,11 @@
       <c r="AW29" s="50">
         <v>10</v>
       </c>
+      <c r="AX29" s="50">
+        <v>11</v>
+      </c>
     </row>
-    <row r="30" spans="1:49" s="12" customFormat="1" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:50" s="12" customFormat="1" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="26" t="s">
         <v>28</v>
       </c>
@@ -6079,8 +6166,11 @@
       <c r="AW30" s="50">
         <v>13</v>
       </c>
+      <c r="AX30" s="50">
+        <v>14</v>
+      </c>
     </row>
-    <row r="31" spans="1:49" s="12" customFormat="1" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:50" s="12" customFormat="1" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" s="26" t="s">
         <v>29</v>
       </c>
@@ -6228,8 +6318,11 @@
       <c r="AW31" s="50">
         <v>8</v>
       </c>
+      <c r="AX31" s="50">
+        <v>10</v>
+      </c>
     </row>
-    <row r="32" spans="1:49" s="12" customFormat="1" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:50" s="12" customFormat="1" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" s="26" t="s">
         <v>30</v>
       </c>
@@ -6377,8 +6470,11 @@
       <c r="AW32" s="50">
         <v>22</v>
       </c>
+      <c r="AX32" s="50">
+        <v>23</v>
+      </c>
     </row>
-    <row r="33" spans="1:49" s="12" customFormat="1" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:50" s="12" customFormat="1" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A33" s="26" t="s">
         <v>31</v>
       </c>
@@ -6526,8 +6622,11 @@
       <c r="AW33" s="50">
         <v>1</v>
       </c>
+      <c r="AX33" s="50">
+        <v>1</v>
+      </c>
     </row>
-    <row r="34" spans="1:49" s="27" customFormat="1" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:50" s="27" customFormat="1" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A34" s="26" t="s">
         <v>32</v>
       </c>
@@ -6675,8 +6774,11 @@
       <c r="AW34" s="50">
         <v>310</v>
       </c>
+      <c r="AX34" s="50">
+        <v>321</v>
+      </c>
     </row>
-    <row r="35" spans="1:49" s="12" customFormat="1" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:50" s="12" customFormat="1" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A35" s="26" t="s">
         <v>33</v>
       </c>
@@ -6824,8 +6926,11 @@
       <c r="AW35" s="50">
         <v>6</v>
       </c>
+      <c r="AX35" s="50">
+        <v>6</v>
+      </c>
     </row>
-    <row r="36" spans="1:49" s="12" customFormat="1" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:50" s="12" customFormat="1" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A36" s="26" t="s">
         <v>34</v>
       </c>
@@ -6973,8 +7078,11 @@
       <c r="AW36" s="50">
         <v>1</v>
       </c>
+      <c r="AX36" s="50">
+        <v>1</v>
+      </c>
     </row>
-    <row r="37" spans="1:49" s="12" customFormat="1" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:50" s="12" customFormat="1" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A37" s="26" t="s">
         <v>35</v>
       </c>
@@ -7122,8 +7230,11 @@
       <c r="AW37" s="50">
         <v>10</v>
       </c>
+      <c r="AX37" s="50">
+        <v>10</v>
+      </c>
     </row>
-    <row r="38" spans="1:49" s="12" customFormat="1" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:50" s="12" customFormat="1" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A38" s="26" t="s">
         <v>36</v>
       </c>
@@ -7271,8 +7382,11 @@
       <c r="AW38" s="50">
         <v>12</v>
       </c>
+      <c r="AX38" s="50">
+        <v>13</v>
+      </c>
     </row>
-    <row r="39" spans="1:49" s="28" customFormat="1" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:50" s="28" customFormat="1" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A39" s="26" t="s">
         <v>37</v>
       </c>
@@ -7420,8 +7534,11 @@
       <c r="AW39" s="50">
         <v>36</v>
       </c>
+      <c r="AX39" s="50">
+        <v>39</v>
+      </c>
     </row>
-    <row r="40" spans="1:49" s="28" customFormat="1" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:50" s="28" customFormat="1" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A40" s="26" t="s">
         <v>38</v>
       </c>
@@ -7569,8 +7686,11 @@
       <c r="AW40" s="50">
         <v>8</v>
       </c>
+      <c r="AX40" s="50">
+        <v>8</v>
+      </c>
     </row>
-    <row r="41" spans="1:49" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:50" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A41" s="26" t="s">
         <v>39</v>
       </c>
@@ -7718,8 +7838,11 @@
       <c r="AW41" s="50">
         <v>1</v>
       </c>
+      <c r="AX41" s="50">
+        <v>1</v>
+      </c>
     </row>
-    <row r="42" spans="1:49" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:50" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A42" s="26" t="s">
         <v>40</v>
       </c>
@@ -7867,8 +7990,11 @@
       <c r="AW42" s="50">
         <v>3</v>
       </c>
+      <c r="AX42" s="50">
+        <v>3</v>
+      </c>
     </row>
-    <row r="43" spans="1:49" s="28" customFormat="1" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:50" s="28" customFormat="1" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A43" s="26" t="s">
         <v>41</v>
       </c>
@@ -8016,8 +8142,11 @@
       <c r="AW43" s="50">
         <v>0</v>
       </c>
+      <c r="AX43" s="50">
+        <v>1</v>
+      </c>
     </row>
-    <row r="44" spans="1:49" s="28" customFormat="1" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:50" s="28" customFormat="1" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A44" s="26" t="s">
         <v>42</v>
       </c>
@@ -8165,8 +8294,11 @@
       <c r="AW44" s="50">
         <v>0</v>
       </c>
+      <c r="AX44" s="50">
+        <v>0</v>
+      </c>
     </row>
-    <row r="45" spans="1:49" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:50" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A45" s="26" t="s">
         <v>43</v>
       </c>
@@ -8314,8 +8446,11 @@
       <c r="AW45" s="50">
         <v>0</v>
       </c>
+      <c r="AX45" s="50">
+        <v>0</v>
+      </c>
     </row>
-    <row r="46" spans="1:49" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:50" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A46" s="26" t="s">
         <v>44</v>
       </c>
@@ -8463,8 +8598,11 @@
       <c r="AW46" s="50">
         <v>570</v>
       </c>
+      <c r="AX46" s="50">
+        <v>584</v>
+      </c>
     </row>
-    <row r="47" spans="1:49" s="28" customFormat="1" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:50" s="28" customFormat="1" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A47" s="26" t="s">
         <v>45</v>
       </c>
@@ -8612,8 +8750,11 @@
       <c r="AW47" s="50">
         <v>0</v>
       </c>
+      <c r="AX47" s="50">
+        <v>0</v>
+      </c>
     </row>
-    <row r="48" spans="1:49" s="28" customFormat="1" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:50" s="28" customFormat="1" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A48" s="26" t="s">
         <v>46</v>
       </c>
@@ -8761,8 +8902,11 @@
       <c r="AW48" s="50">
         <v>9</v>
       </c>
+      <c r="AX48" s="50">
+        <v>10</v>
+      </c>
     </row>
-    <row r="49" spans="1:49" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:50" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A49" s="26" t="s">
         <v>47</v>
       </c>
@@ -8910,8 +9054,11 @@
       <c r="AW49" s="50">
         <v>45</v>
       </c>
+      <c r="AX49" s="50">
+        <v>47</v>
+      </c>
     </row>
-    <row r="50" spans="1:49" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:50" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A50" s="26" t="s">
         <v>48</v>
       </c>
@@ -9059,8 +9206,11 @@
       <c r="AW50" s="50">
         <v>3</v>
       </c>
+      <c r="AX50" s="50">
+        <v>3</v>
+      </c>
     </row>
-    <row r="51" spans="1:49" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:50" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A51" s="26" t="s">
         <v>49</v>
       </c>
@@ -9208,8 +9358,11 @@
       <c r="AW51" s="50">
         <v>1</v>
       </c>
+      <c r="AX51" s="50">
+        <v>1</v>
+      </c>
     </row>
-    <row r="52" spans="1:49" s="28" customFormat="1" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:50" s="28" customFormat="1" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A52" s="26" t="s">
         <v>50</v>
       </c>
@@ -9357,8 +9510,11 @@
       <c r="AW52" s="50">
         <v>4</v>
       </c>
+      <c r="AX52" s="50">
+        <v>4</v>
+      </c>
     </row>
-    <row r="53" spans="1:49" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:50" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A53" s="26" t="s">
         <v>51</v>
       </c>
@@ -9506,8 +9662,11 @@
       <c r="AW53" s="50">
         <v>86</v>
       </c>
+      <c r="AX53" s="50">
+        <v>86</v>
+      </c>
     </row>
-    <row r="54" spans="1:49" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:50" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A54" s="26" t="s">
         <v>52</v>
       </c>
@@ -9655,8 +9814,11 @@
       <c r="AW54" s="50">
         <v>0</v>
       </c>
+      <c r="AX54" s="50">
+        <v>0</v>
+      </c>
     </row>
-    <row r="55" spans="1:49" s="28" customFormat="1" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:50" s="28" customFormat="1" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A55" s="26" t="s">
         <v>53</v>
       </c>
@@ -9804,8 +9966,11 @@
       <c r="AW55" s="50">
         <v>2</v>
       </c>
+      <c r="AX55" s="50">
+        <v>2</v>
+      </c>
     </row>
-    <row r="56" spans="1:49" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:50" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A56" s="26" t="s">
         <v>54</v>
       </c>
@@ -9953,8 +10118,11 @@
       <c r="AW56" s="50">
         <v>0</v>
       </c>
+      <c r="AX56" s="50">
+        <v>0</v>
+      </c>
     </row>
-    <row r="57" spans="1:49" s="28" customFormat="1" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:50" s="28" customFormat="1" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A57" s="26" t="s">
         <v>55</v>
       </c>
@@ -10102,8 +10270,11 @@
       <c r="AW57" s="50">
         <v>1</v>
       </c>
+      <c r="AX57" s="50">
+        <v>1</v>
+      </c>
     </row>
-    <row r="58" spans="1:49" s="28" customFormat="1" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:50" s="28" customFormat="1" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A58" s="26" t="s">
         <v>56</v>
       </c>
@@ -10251,8 +10422,11 @@
       <c r="AW58" s="50">
         <v>0</v>
       </c>
+      <c r="AX58" s="50">
+        <v>0</v>
+      </c>
     </row>
-    <row r="59" spans="1:49" s="28" customFormat="1" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:50" s="28" customFormat="1" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A59" s="26" t="s">
         <v>57</v>
       </c>
@@ -10400,8 +10574,11 @@
       <c r="AW59" s="50">
         <v>3</v>
       </c>
+      <c r="AX59" s="50">
+        <v>3</v>
+      </c>
     </row>
-    <row r="60" spans="1:49" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:50" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A60" s="26" t="s">
         <v>58</v>
       </c>
@@ -10549,8 +10726,11 @@
       <c r="AW60" s="50">
         <v>2602</v>
       </c>
+      <c r="AX60" s="50">
+        <v>2683</v>
+      </c>
     </row>
-    <row r="61" spans="1:49" s="28" customFormat="1" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:50" s="28" customFormat="1" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A61" s="26" t="s">
         <v>59</v>
       </c>
@@ -10698,8 +10878,11 @@
       <c r="AW61" s="50">
         <v>14</v>
       </c>
+      <c r="AX61" s="50">
+        <v>18</v>
+      </c>
     </row>
-    <row r="62" spans="1:49" s="28" customFormat="1" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:50" s="28" customFormat="1" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A62" s="26" t="s">
         <v>60</v>
       </c>
@@ -10847,8 +11030,11 @@
       <c r="AW62" s="50">
         <v>14</v>
       </c>
+      <c r="AX62" s="50">
+        <v>17</v>
+      </c>
     </row>
-    <row r="63" spans="1:49" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:50" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A63" s="26" t="s">
         <v>61</v>
       </c>
@@ -10996,8 +11182,11 @@
       <c r="AW63" s="50">
         <v>1</v>
       </c>
+      <c r="AX63" s="50">
+        <v>1</v>
+      </c>
     </row>
-    <row r="64" spans="1:49" s="28" customFormat="1" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:50" s="28" customFormat="1" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A64" s="26" t="s">
         <v>62</v>
       </c>
@@ -11145,8 +11334,11 @@
       <c r="AW64" s="50">
         <v>619</v>
       </c>
+      <c r="AX64" s="50">
+        <v>644</v>
+      </c>
     </row>
-    <row r="65" spans="1:49" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:50" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A65" s="26" t="s">
         <v>63</v>
       </c>
@@ -11294,8 +11486,11 @@
       <c r="AW65" s="50">
         <v>14</v>
       </c>
+      <c r="AX65" s="50">
+        <v>14</v>
+      </c>
     </row>
-    <row r="66" spans="1:49" s="28" customFormat="1" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:50" s="28" customFormat="1" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A66" s="26" t="s">
         <v>64</v>
       </c>
@@ -11443,8 +11638,11 @@
       <c r="AW66" s="50">
         <v>1</v>
       </c>
+      <c r="AX66" s="50">
+        <v>1</v>
+      </c>
     </row>
-    <row r="67" spans="1:49" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:50" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A67" s="26" t="s">
         <v>65</v>
       </c>
@@ -11592,8 +11790,11 @@
       <c r="AW67" s="50">
         <v>1</v>
       </c>
+      <c r="AX67" s="50">
+        <v>1</v>
+      </c>
     </row>
-    <row r="68" spans="1:49" s="28" customFormat="1" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:50" s="28" customFormat="1" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A68" s="26" t="s">
         <v>66</v>
       </c>
@@ -11741,8 +11942,11 @@
       <c r="AW68" s="50">
         <v>24</v>
       </c>
+      <c r="AX68" s="50">
+        <v>24</v>
+      </c>
     </row>
-    <row r="69" spans="1:49" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:50" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A69" s="26" t="s">
         <v>67</v>
       </c>
@@ -11890,8 +12094,11 @@
       <c r="AW69" s="50">
         <v>1</v>
       </c>
+      <c r="AX69" s="50">
+        <v>1</v>
+      </c>
     </row>
-    <row r="70" spans="1:49" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:50" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A70" s="26" t="s">
         <v>68</v>
       </c>
@@ -12039,8 +12246,11 @@
       <c r="AW70" s="50">
         <v>3</v>
       </c>
+      <c r="AX70" s="50">
+        <v>3</v>
+      </c>
     </row>
-    <row r="71" spans="1:49" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:50" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A71" s="26" t="s">
         <v>69</v>
       </c>
@@ -12188,8 +12398,11 @@
       <c r="AW71" s="50">
         <v>61</v>
       </c>
+      <c r="AX71" s="50">
+        <v>62</v>
+      </c>
     </row>
-    <row r="72" spans="1:49" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:50" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A72" s="26" t="s">
         <v>70</v>
       </c>
@@ -12337,8 +12550,11 @@
       <c r="AW72" s="50">
         <v>0</v>
       </c>
+      <c r="AX72" s="50">
+        <v>0</v>
+      </c>
     </row>
-    <row r="73" spans="1:49" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:50" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A73" s="26" t="s">
         <v>71</v>
       </c>
@@ -12486,8 +12702,11 @@
       <c r="AW73" s="50">
         <v>110</v>
       </c>
+      <c r="AX73" s="50">
+        <v>111</v>
+      </c>
     </row>
-    <row r="74" spans="1:49" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:50" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A74" s="26" t="s">
         <v>72</v>
       </c>
@@ -12635,8 +12854,11 @@
       <c r="AW74" s="50">
         <v>587</v>
       </c>
+      <c r="AX74" s="50">
+        <v>645</v>
+      </c>
     </row>
-    <row r="75" spans="1:49" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:50" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A75" s="26" t="s">
         <v>73</v>
       </c>
@@ -12784,8 +13006,11 @@
       <c r="AW75" s="50">
         <v>12</v>
       </c>
+      <c r="AX75" s="50">
+        <v>12</v>
+      </c>
     </row>
-    <row r="76" spans="1:49" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:50" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A76" s="26" t="s">
         <v>74</v>
       </c>
@@ -12933,8 +13158,11 @@
       <c r="AW76" s="50">
         <v>1</v>
       </c>
+      <c r="AX76" s="50">
+        <v>1</v>
+      </c>
     </row>
-    <row r="77" spans="1:49" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:50" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A77" s="26" t="s">
         <v>75</v>
       </c>
@@ -13082,8 +13310,11 @@
       <c r="AW77" s="50">
         <v>12</v>
       </c>
+      <c r="AX77" s="50">
+        <v>13</v>
+      </c>
     </row>
-    <row r="78" spans="1:49" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:50" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A78" s="26" t="s">
         <v>76</v>
       </c>
@@ -13231,8 +13462,11 @@
       <c r="AW78" s="50">
         <v>15</v>
       </c>
+      <c r="AX78" s="50">
+        <v>15</v>
+      </c>
     </row>
-    <row r="79" spans="1:49" s="29" customFormat="1" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:50" s="29" customFormat="1" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A79" s="26" t="s">
         <v>77</v>
       </c>
@@ -13380,8 +13614,11 @@
       <c r="AW79" s="50">
         <v>0</v>
       </c>
+      <c r="AX79" s="50">
+        <v>0</v>
+      </c>
     </row>
-    <row r="80" spans="1:49" s="29" customFormat="1" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:50" s="29" customFormat="1" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A80" s="26" t="s">
         <v>78</v>
       </c>
@@ -13529,8 +13766,11 @@
       <c r="AW80" s="50">
         <v>2</v>
       </c>
+      <c r="AX80" s="50">
+        <v>3</v>
+      </c>
     </row>
-    <row r="81" spans="1:49" s="29" customFormat="1" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:50" s="29" customFormat="1" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A81" s="26" t="s">
         <v>79</v>
       </c>
@@ -13678,8 +13918,11 @@
       <c r="AW81" s="50">
         <v>0</v>
       </c>
+      <c r="AX81" s="50">
+        <v>0</v>
+      </c>
     </row>
-    <row r="82" spans="1:49" s="29" customFormat="1" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:50" s="29" customFormat="1" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A82" s="26" t="s">
         <v>80</v>
       </c>
@@ -13827,8 +14070,11 @@
       <c r="AW82" s="50">
         <v>808</v>
       </c>
+      <c r="AX82" s="50">
+        <v>870</v>
+      </c>
     </row>
-    <row r="83" spans="1:49" s="29" customFormat="1" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:50" s="29" customFormat="1" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A83" s="26" t="s">
         <v>81</v>
       </c>
@@ -13976,8 +14222,11 @@
       <c r="AW83" s="50">
         <v>1</v>
       </c>
+      <c r="AX83" s="50">
+        <v>1</v>
+      </c>
     </row>
-    <row r="84" spans="1:49" s="29" customFormat="1" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:50" s="29" customFormat="1" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A84" s="26" t="s">
         <v>82</v>
       </c>
@@ -14125,8 +14374,11 @@
       <c r="AW84" s="50">
         <v>3</v>
       </c>
+      <c r="AX84" s="50">
+        <v>3</v>
+      </c>
     </row>
-    <row r="85" spans="1:49" s="29" customFormat="1" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:50" s="29" customFormat="1" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A85" s="26" t="s">
         <v>83</v>
       </c>
@@ -14274,8 +14526,11 @@
       <c r="AW85" s="50">
         <v>1</v>
       </c>
+      <c r="AX85" s="50">
+        <v>1</v>
+      </c>
     </row>
-    <row r="86" spans="1:49" s="29" customFormat="1" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:50" s="29" customFormat="1" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A86" s="26" t="s">
         <v>84</v>
       </c>
@@ -14423,8 +14678,11 @@
       <c r="AW86" s="50">
         <v>2</v>
       </c>
+      <c r="AX86" s="50">
+        <v>2</v>
+      </c>
     </row>
-    <row r="87" spans="1:49" s="29" customFormat="1" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:50" s="29" customFormat="1" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A87" s="26" t="s">
         <v>85</v>
       </c>
@@ -14572,8 +14830,11 @@
       <c r="AW87" s="50">
         <v>479</v>
       </c>
+      <c r="AX87" s="50">
+        <v>491</v>
+      </c>
     </row>
-    <row r="88" spans="1:49" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:50" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A88" s="26" t="s">
         <v>86</v>
       </c>
@@ -14721,8 +14982,11 @@
       <c r="AW88" s="50">
         <v>0</v>
       </c>
+      <c r="AX88" s="50">
+        <v>0</v>
+      </c>
     </row>
-    <row r="89" spans="1:49" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:50" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A89" s="26" t="s">
         <v>87</v>
       </c>
@@ -14870,8 +15134,11 @@
       <c r="AW89" s="50">
         <v>1</v>
       </c>
+      <c r="AX89" s="50">
+        <v>1</v>
+      </c>
     </row>
-    <row r="90" spans="1:49" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:50" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A90" s="26" t="s">
         <v>88</v>
       </c>
@@ -15019,8 +15286,11 @@
       <c r="AW90" s="50">
         <v>0</v>
       </c>
+      <c r="AX90" s="50">
+        <v>0</v>
+      </c>
     </row>
-    <row r="91" spans="1:49" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:50" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A91" s="26" t="s">
         <v>89</v>
       </c>
@@ -15168,8 +15438,11 @@
       <c r="AW91" s="50">
         <v>6</v>
       </c>
+      <c r="AX91" s="50">
+        <v>6</v>
+      </c>
     </row>
-    <row r="92" spans="1:49" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:50" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A92" s="26" t="s">
         <v>90</v>
       </c>
@@ -15317,8 +15590,11 @@
       <c r="AW92" s="50">
         <v>3</v>
       </c>
+      <c r="AX92" s="50">
+        <v>4</v>
+      </c>
     </row>
-    <row r="93" spans="1:49" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:50" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A93" s="26" t="s">
         <v>91</v>
       </c>
@@ -15466,8 +15742,11 @@
       <c r="AW93" s="50">
         <v>22</v>
       </c>
+      <c r="AX93" s="50">
+        <v>27</v>
+      </c>
     </row>
-    <row r="94" spans="1:49" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:50" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A94" s="26" t="s">
         <v>92</v>
       </c>
@@ -15615,8 +15894,11 @@
       <c r="AW94" s="50">
         <v>19</v>
       </c>
+      <c r="AX94" s="50">
+        <v>19</v>
+      </c>
     </row>
-    <row r="95" spans="1:49" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:50" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A95" s="26" t="s">
         <v>93</v>
       </c>
@@ -15764,8 +16046,11 @@
       <c r="AW95" s="50">
         <v>53</v>
       </c>
+      <c r="AX95" s="50">
+        <v>55</v>
+      </c>
     </row>
-    <row r="96" spans="1:49" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:50" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A96" s="26" t="s">
         <v>94</v>
       </c>
@@ -15913,8 +16198,11 @@
       <c r="AW96" s="50">
         <v>10</v>
       </c>
+      <c r="AX96" s="50">
+        <v>10</v>
+      </c>
     </row>
-    <row r="97" spans="1:49" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:50" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A97" s="26" t="s">
         <v>95</v>
       </c>
@@ -16062,8 +16350,11 @@
       <c r="AW97" s="50">
         <v>63</v>
       </c>
+      <c r="AX97" s="50">
+        <v>64</v>
+      </c>
     </row>
-    <row r="98" spans="1:49" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:50" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A98" s="26" t="s">
         <v>96</v>
       </c>
@@ -16211,8 +16502,11 @@
       <c r="AW98" s="50">
         <v>16</v>
       </c>
+      <c r="AX98" s="50">
+        <v>16</v>
+      </c>
     </row>
-    <row r="99" spans="1:49" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:50" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A99" s="26" t="s">
         <v>97</v>
       </c>
@@ -16360,8 +16654,11 @@
       <c r="AW99" s="50">
         <v>0</v>
       </c>
+      <c r="AX99" s="50">
+        <v>0</v>
+      </c>
     </row>
-    <row r="100" spans="1:49" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:50" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A100" s="26" t="s">
         <v>98</v>
       </c>
@@ -16509,8 +16806,11 @@
       <c r="AW100" s="50">
         <v>5</v>
       </c>
+      <c r="AX100" s="50">
+        <v>5</v>
+      </c>
     </row>
-    <row r="101" spans="1:49" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:50" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A101" s="26" t="s">
         <v>99</v>
       </c>
@@ -16658,8 +16958,11 @@
       <c r="AW101" s="50">
         <v>1</v>
       </c>
+      <c r="AX101" s="50">
+        <v>2</v>
+      </c>
     </row>
-    <row r="102" spans="1:49" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:50" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A102" s="26" t="s">
         <v>100</v>
       </c>
@@ -16807,8 +17110,11 @@
       <c r="AW102" s="50">
         <v>0</v>
       </c>
+      <c r="AX102" s="50">
+        <v>0</v>
+      </c>
     </row>
-    <row r="103" spans="1:49" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:50" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A103" s="26" t="s">
         <v>101</v>
       </c>
@@ -16956,8 +17262,11 @@
       <c r="AW103" s="50">
         <v>89</v>
       </c>
+      <c r="AX103" s="50">
+        <v>91</v>
+      </c>
     </row>
-    <row r="104" spans="1:49" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:50" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A104" s="26" t="s">
         <v>102</v>
       </c>
@@ -17105,8 +17414,11 @@
       <c r="AW104" s="50">
         <v>5143</v>
       </c>
+      <c r="AX104" s="50">
+        <v>5211</v>
+      </c>
     </row>
-    <row r="105" spans="1:49" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:50" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A105" s="26" t="s">
         <v>103</v>
       </c>
@@ -17254,8 +17566,11 @@
       <c r="AW105" s="50">
         <v>59</v>
       </c>
+      <c r="AX105" s="50">
+        <v>61</v>
+      </c>
     </row>
-    <row r="106" spans="1:49" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:50" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A106" s="26" t="s">
         <v>104</v>
       </c>
@@ -17403,8 +17718,11 @@
       <c r="AW106" s="50">
         <v>1</v>
       </c>
+      <c r="AX106" s="50">
+        <v>2</v>
+      </c>
     </row>
-    <row r="107" spans="1:49" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:50" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A107" s="26" t="s">
         <v>105</v>
       </c>
@@ -17552,8 +17870,11 @@
       <c r="AW107" s="50">
         <v>0</v>
       </c>
+      <c r="AX107" s="50">
+        <v>0</v>
+      </c>
     </row>
-    <row r="108" spans="1:49" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:50" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A108" s="26" t="s">
         <v>106</v>
       </c>
@@ -17701,8 +18022,11 @@
       <c r="AW108" s="50">
         <v>140</v>
       </c>
+      <c r="AX108" s="50">
+        <v>140</v>
+      </c>
     </row>
-    <row r="109" spans="1:49" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:50" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A109" s="26" t="s">
         <v>107</v>
       </c>
@@ -17850,8 +18174,11 @@
       <c r="AW109" s="50">
         <v>1</v>
       </c>
+      <c r="AX109" s="50">
+        <v>1</v>
+      </c>
     </row>
-    <row r="110" spans="1:49" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:50" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A110" s="26" t="s">
         <v>108</v>
       </c>
@@ -17999,8 +18326,11 @@
       <c r="AW110" s="50">
         <v>19</v>
       </c>
+      <c r="AX110" s="50">
+        <v>22</v>
+      </c>
     </row>
-    <row r="111" spans="1:49" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:50" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A111" s="26" t="s">
         <v>109</v>
       </c>
@@ -18148,8 +18478,11 @@
       <c r="AW111" s="50">
         <v>275</v>
       </c>
+      <c r="AX111" s="50">
+        <v>281</v>
+      </c>
     </row>
-    <row r="112" spans="1:49" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:50" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A112" s="26" t="s">
         <v>110</v>
       </c>
@@ -18297,8 +18630,11 @@
       <c r="AW112" s="50">
         <v>12</v>
       </c>
+      <c r="AX112" s="50">
+        <v>14</v>
+      </c>
     </row>
-    <row r="113" spans="1:49" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:50" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A113" s="26" t="s">
         <v>111</v>
       </c>
@@ -18446,8 +18782,11 @@
       <c r="AW113" s="50">
         <v>17</v>
       </c>
+      <c r="AX113" s="50">
+        <v>18</v>
+      </c>
     </row>
-    <row r="114" spans="1:49" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:50" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A114" s="26" t="s">
         <v>112</v>
       </c>
@@ -18595,8 +18934,11 @@
       <c r="AW114" s="50">
         <v>15</v>
       </c>
+      <c r="AX114" s="50">
+        <v>15</v>
+      </c>
     </row>
-    <row r="115" spans="1:49" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:50" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A115" s="26" t="s">
         <v>113</v>
       </c>
@@ -18744,8 +19086,11 @@
       <c r="AW115" s="50">
         <v>4</v>
       </c>
+      <c r="AX115" s="50">
+        <v>4</v>
+      </c>
     </row>
-    <row r="116" spans="1:49" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:50" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A116" s="26" t="s">
         <v>114</v>
       </c>
@@ -18893,8 +19238,11 @@
       <c r="AW116" s="50">
         <v>1</v>
       </c>
+      <c r="AX116" s="50">
+        <v>4</v>
+      </c>
     </row>
-    <row r="117" spans="1:49" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:50" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A117" s="26" t="s">
         <v>115</v>
       </c>
@@ -19042,8 +19390,11 @@
       <c r="AW117" s="50">
         <v>1</v>
       </c>
+      <c r="AX117" s="50">
+        <v>2</v>
+      </c>
     </row>
-    <row r="118" spans="1:49" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:50" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A118" s="26" t="s">
         <v>116</v>
       </c>
@@ -19191,8 +19542,11 @@
       <c r="AW118" s="50">
         <v>0</v>
       </c>
+      <c r="AX118" s="50">
+        <v>0</v>
+      </c>
     </row>
-    <row r="119" spans="1:49" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:50" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A119" s="26" t="s">
         <v>117</v>
       </c>
@@ -19340,8 +19694,11 @@
       <c r="AW119" s="50">
         <v>38</v>
       </c>
+      <c r="AX119" s="50">
+        <v>37</v>
+      </c>
     </row>
-    <row r="120" spans="1:49" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:50" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A120" s="26" t="s">
         <v>118</v>
       </c>
@@ -19489,8 +19846,11 @@
       <c r="AW120" s="50">
         <v>8</v>
       </c>
+      <c r="AX120" s="50">
+        <v>9</v>
+      </c>
     </row>
-    <row r="121" spans="1:49" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:50" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A121" s="26" t="s">
         <v>119</v>
       </c>
@@ -19638,8 +19998,11 @@
       <c r="AW121" s="50">
         <v>0</v>
       </c>
+      <c r="AX121" s="50">
+        <v>0</v>
+      </c>
     </row>
-    <row r="122" spans="1:49" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:50" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A122" s="26" t="s">
         <v>120</v>
       </c>
@@ -19787,8 +20150,11 @@
       <c r="AW122" s="50">
         <v>4</v>
       </c>
+      <c r="AX122" s="50">
+        <v>4</v>
+      </c>
     </row>
-    <row r="123" spans="1:49" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:50" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A123" s="26" t="s">
         <v>121</v>
       </c>
@@ -19936,8 +20302,11 @@
       <c r="AW123" s="50">
         <v>6</v>
       </c>
+      <c r="AX123" s="50">
+        <v>6</v>
+      </c>
     </row>
-    <row r="124" spans="1:49" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:50" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A124" s="26" t="s">
         <v>122</v>
       </c>
@@ -20085,8 +20454,11 @@
       <c r="AW124" s="50">
         <v>10</v>
       </c>
+      <c r="AX124" s="50">
+        <v>10</v>
+      </c>
     </row>
-    <row r="125" spans="1:49" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:50" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A125" s="26" t="s">
         <v>123</v>
       </c>
@@ -20234,8 +20606,11 @@
       <c r="AW125" s="50">
         <v>0</v>
       </c>
+      <c r="AX125" s="50">
+        <v>0</v>
+      </c>
     </row>
-    <row r="126" spans="1:49" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:50" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A126" s="26" t="s">
         <v>124</v>
       </c>
@@ -20383,8 +20758,11 @@
       <c r="AW126" s="50">
         <v>209</v>
       </c>
+      <c r="AX126" s="50">
+        <v>224</v>
+      </c>
     </row>
-    <row r="127" spans="1:49" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:50" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A127" s="26" t="s">
         <v>125</v>
       </c>
@@ -20532,8 +20910,11 @@
       <c r="AW127" s="50">
         <v>0</v>
       </c>
+      <c r="AX127" s="50">
+        <v>1</v>
+      </c>
     </row>
-    <row r="128" spans="1:49" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:50" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A128" s="26" t="s">
         <v>126</v>
       </c>
@@ -20681,8 +21062,11 @@
       <c r="AW128" s="50">
         <v>2</v>
       </c>
+      <c r="AX128" s="50">
+        <v>2</v>
+      </c>
     </row>
-    <row r="129" spans="1:49" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:50" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A129" s="26" t="s">
         <v>127</v>
       </c>
@@ -20830,8 +21214,11 @@
       <c r="AW129" s="50">
         <v>47</v>
       </c>
+      <c r="AX129" s="50">
+        <v>50</v>
+      </c>
     </row>
-    <row r="130" spans="1:49" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:50" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A130" s="26" t="s">
         <v>128</v>
       </c>
@@ -20979,8 +21366,11 @@
       <c r="AW130" s="50">
         <v>3</v>
       </c>
+      <c r="AX130" s="50">
+        <v>4</v>
+      </c>
     </row>
-    <row r="131" spans="1:49" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:50" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A131" s="26" t="s">
         <v>129</v>
       </c>
@@ -21128,8 +21518,11 @@
       <c r="AW131" s="50">
         <v>3</v>
       </c>
+      <c r="AX131" s="50">
+        <v>3</v>
+      </c>
     </row>
-    <row r="132" spans="1:49" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:50" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A132" s="26" t="s">
         <v>130</v>
       </c>
@@ -21277,8 +21670,11 @@
       <c r="AW132" s="50">
         <v>51</v>
       </c>
+      <c r="AX132" s="50">
+        <v>58</v>
+      </c>
     </row>
-    <row r="133" spans="1:49" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:50" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A133" s="26" t="s">
         <v>131</v>
       </c>
@@ -21426,8 +21822,11 @@
       <c r="AW133" s="50">
         <v>14</v>
       </c>
+      <c r="AX133" s="50">
+        <v>15</v>
+      </c>
     </row>
-    <row r="134" spans="1:49" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:50" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A134" s="26" t="s">
         <v>132</v>
       </c>
@@ -21575,8 +21974,11 @@
       <c r="AW134" s="50">
         <v>0</v>
       </c>
+      <c r="AX134" s="50">
+        <v>0</v>
+      </c>
     </row>
-    <row r="135" spans="1:49" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:50" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A135" s="26" t="s">
         <v>133</v>
       </c>
@@ -21724,8 +22126,11 @@
       <c r="AW135" s="50">
         <v>0</v>
       </c>
+      <c r="AX135" s="50">
+        <v>0</v>
+      </c>
     </row>
-    <row r="136" spans="1:49" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:50" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A136" s="26" t="s">
         <v>134</v>
       </c>
@@ -21873,8 +22278,11 @@
       <c r="AW136" s="50">
         <v>4</v>
       </c>
+      <c r="AX136" s="50">
+        <v>5</v>
+      </c>
     </row>
-    <row r="137" spans="1:49" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:50" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A137" s="26" t="s">
         <v>135</v>
       </c>
@@ -22022,8 +22430,11 @@
       <c r="AW137" s="50">
         <v>0</v>
       </c>
+      <c r="AX137" s="50">
+        <v>0</v>
+      </c>
     </row>
-    <row r="138" spans="1:49" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:50" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A138" s="26" t="s">
         <v>136</v>
       </c>
@@ -22171,8 +22582,11 @@
       <c r="AW138" s="50">
         <v>0</v>
       </c>
+      <c r="AX138" s="50">
+        <v>0</v>
+      </c>
     </row>
-    <row r="139" spans="1:49" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:50" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A139" s="26" t="s">
         <v>137</v>
       </c>
@@ -22320,8 +22734,11 @@
       <c r="AW139" s="50">
         <v>0</v>
       </c>
+      <c r="AX139" s="50">
+        <v>0</v>
+      </c>
     </row>
-    <row r="140" spans="1:49" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:50" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A140" s="26" t="s">
         <v>138</v>
       </c>
@@ -22469,8 +22886,11 @@
       <c r="AW140" s="50">
         <v>7</v>
       </c>
+      <c r="AX140" s="50">
+        <v>7</v>
+      </c>
     </row>
-    <row r="141" spans="1:49" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:50" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A141" s="26" t="s">
         <v>139</v>
       </c>
@@ -22618,8 +23038,11 @@
       <c r="AW141" s="50">
         <v>1</v>
       </c>
+      <c r="AX141" s="50">
+        <v>1</v>
+      </c>
     </row>
-    <row r="142" spans="1:49" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:50" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A142" s="26" t="s">
         <v>140</v>
       </c>
@@ -22767,8 +23190,11 @@
       <c r="AW142" s="50">
         <v>8</v>
       </c>
+      <c r="AX142" s="50">
+        <v>7</v>
+      </c>
     </row>
-    <row r="143" spans="1:49" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:50" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A143" s="26" t="s">
         <v>141</v>
       </c>
@@ -22916,8 +23342,11 @@
       <c r="AW143" s="50">
         <v>2</v>
       </c>
+      <c r="AX143" s="50">
+        <v>2</v>
+      </c>
     </row>
-    <row r="144" spans="1:49" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:50" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A144" s="26" t="s">
         <v>142</v>
       </c>
@@ -23065,8 +23494,11 @@
       <c r="AW144" s="50">
         <v>2</v>
       </c>
+      <c r="AX144" s="50">
+        <v>2</v>
+      </c>
     </row>
-    <row r="145" spans="1:49" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:50" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A145" s="26" t="s">
         <v>143</v>
       </c>
@@ -23214,8 +23646,11 @@
       <c r="AW145" s="50">
         <v>1</v>
       </c>
+      <c r="AX145" s="50">
+        <v>1</v>
+      </c>
     </row>
-    <row r="146" spans="1:49" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:50" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A146" s="26" t="s">
         <v>144</v>
       </c>
@@ -23363,8 +23798,11 @@
       <c r="AW146" s="50">
         <v>4</v>
       </c>
+      <c r="AX146" s="50">
+        <v>5</v>
+      </c>
     </row>
-    <row r="147" spans="1:49" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:50" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A147" s="26" t="s">
         <v>145</v>
       </c>
@@ -23512,8 +23950,11 @@
       <c r="AW147" s="50">
         <v>2</v>
       </c>
+      <c r="AX147" s="50">
+        <v>2</v>
+      </c>
     </row>
-    <row r="148" spans="1:49" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:50" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A148" s="26" t="s">
         <v>146</v>
       </c>
@@ -23661,8 +24102,11 @@
       <c r="AW148" s="50">
         <v>5</v>
       </c>
+      <c r="AX148" s="50">
+        <v>5</v>
+      </c>
     </row>
-    <row r="149" spans="1:49" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:50" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A149" s="26" t="s">
         <v>147</v>
       </c>
@@ -23810,8 +24254,11 @@
       <c r="AW149" s="50">
         <v>37</v>
       </c>
+      <c r="AX149" s="50">
+        <v>36</v>
+      </c>
     </row>
-    <row r="150" spans="1:49" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:50" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A150" s="26" t="s">
         <v>148</v>
       </c>
@@ -23959,8 +24406,11 @@
       <c r="AW150" s="50">
         <v>11</v>
       </c>
+      <c r="AX150" s="50">
+        <v>11</v>
+      </c>
     </row>
-    <row r="151" spans="1:49" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:50" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A151" s="26" t="s">
         <v>149</v>
       </c>
@@ -24108,8 +24558,11 @@
       <c r="AW151" s="50">
         <v>0</v>
       </c>
+      <c r="AX151" s="50">
+        <v>0</v>
+      </c>
     </row>
-    <row r="152" spans="1:49" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:50" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A152" s="26" t="s">
         <v>150</v>
       </c>
@@ -24257,8 +24710,11 @@
       <c r="AW152" s="50">
         <v>5</v>
       </c>
+      <c r="AX152" s="50">
+        <v>5</v>
+      </c>
     </row>
-    <row r="153" spans="1:49" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:50" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A153" s="26" t="s">
         <v>151</v>
       </c>
@@ -24406,8 +24862,11 @@
       <c r="AW153" s="50">
         <v>3</v>
       </c>
+      <c r="AX153" s="50">
+        <v>3</v>
+      </c>
     </row>
-    <row r="154" spans="1:49" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:50" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A154" s="26" t="s">
         <v>152</v>
       </c>
@@ -24555,8 +25014,11 @@
       <c r="AW154" s="50">
         <v>0</v>
       </c>
+      <c r="AX154" s="50">
+        <v>0</v>
+      </c>
     </row>
-    <row r="155" spans="1:49" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:50" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A155" s="26" t="s">
         <v>153</v>
       </c>
@@ -24704,8 +25166,11 @@
       <c r="AW155" s="50">
         <v>458</v>
       </c>
+      <c r="AX155" s="50">
+        <v>470</v>
+      </c>
     </row>
-    <row r="156" spans="1:49" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:50" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A156" s="26" t="s">
         <v>154</v>
       </c>
@@ -24853,8 +25318,11 @@
       <c r="AW156" s="50">
         <v>5</v>
       </c>
+      <c r="AX156" s="50">
+        <v>5</v>
+      </c>
     </row>
-    <row r="157" spans="1:49" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:50" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A157" s="26" t="s">
         <v>155</v>
       </c>
@@ -25002,8 +25470,11 @@
       <c r="AW157" s="50">
         <v>3</v>
       </c>
+      <c r="AX157" s="50">
+        <v>3</v>
+      </c>
     </row>
-    <row r="158" spans="1:49" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:50" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A158" s="26" t="s">
         <v>156</v>
       </c>
@@ -25151,8 +25622,11 @@
       <c r="AW158" s="50">
         <v>78</v>
       </c>
+      <c r="AX158" s="50">
+        <v>81</v>
+      </c>
     </row>
-    <row r="159" spans="1:49" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:50" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A159" s="26" t="s">
         <v>157</v>
       </c>
@@ -25300,8 +25774,11 @@
       <c r="AW159" s="50">
         <v>0</v>
       </c>
+      <c r="AX159" s="50">
+        <v>0</v>
+      </c>
     </row>
-    <row r="160" spans="1:49" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:50" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A160" s="26" t="s">
         <v>158</v>
       </c>
@@ -25449,8 +25926,11 @@
       <c r="AW160" s="50">
         <v>2</v>
       </c>
+      <c r="AX160" s="50">
+        <v>2</v>
+      </c>
     </row>
-    <row r="161" spans="1:49" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:50" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A161" s="26" t="s">
         <v>159</v>
       </c>
@@ -25598,8 +26078,11 @@
       <c r="AW161" s="50">
         <v>6</v>
       </c>
+      <c r="AX161" s="50">
+        <v>6</v>
+      </c>
     </row>
-    <row r="162" spans="1:49" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="162" spans="1:50" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A162" s="26" t="s">
         <v>160</v>
       </c>
@@ -25747,8 +26230,11 @@
       <c r="AW162" s="50">
         <v>2</v>
       </c>
+      <c r="AX162" s="50">
+        <v>2</v>
+      </c>
     </row>
-    <row r="163" spans="1:49" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="163" spans="1:50" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A163" s="26" t="s">
         <v>161</v>
       </c>
@@ -25896,8 +26382,11 @@
       <c r="AW163" s="50">
         <v>1</v>
       </c>
+      <c r="AX163" s="50">
+        <v>1</v>
+      </c>
     </row>
-    <row r="164" spans="1:49" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:50" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A164" s="26" t="s">
         <v>162</v>
       </c>
@@ -26045,8 +26534,11 @@
       <c r="AW164" s="50">
         <v>55</v>
       </c>
+      <c r="AX164" s="50">
+        <v>57</v>
+      </c>
     </row>
-    <row r="165" spans="1:49" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="165" spans="1:50" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A165" s="26" t="s">
         <v>163</v>
       </c>
@@ -26194,8 +26686,11 @@
       <c r="AW165" s="50">
         <v>15</v>
       </c>
+      <c r="AX165" s="50">
+        <v>14</v>
+      </c>
     </row>
-    <row r="166" spans="1:49" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:50" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A166" s="26" t="s">
         <v>164</v>
       </c>
@@ -26343,8 +26838,11 @@
       <c r="AW166" s="50">
         <v>17</v>
       </c>
+      <c r="AX166" s="50">
+        <v>17</v>
+      </c>
     </row>
-    <row r="167" spans="1:49" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:50" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A167" s="26" t="s">
         <v>165</v>
       </c>
@@ -26492,8 +26990,11 @@
       <c r="AW167" s="50">
         <v>0</v>
       </c>
+      <c r="AX167" s="50">
+        <v>0</v>
+      </c>
     </row>
-    <row r="168" spans="1:49" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="168" spans="1:50" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A168" s="26" t="s">
         <v>166</v>
       </c>
@@ -26641,8 +27142,11 @@
       <c r="AW168" s="50">
         <v>65</v>
       </c>
+      <c r="AX168" s="50">
+        <v>67</v>
+      </c>
     </row>
-    <row r="169" spans="1:49" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="169" spans="1:50" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A169" s="26" t="s">
         <v>167</v>
       </c>
@@ -26790,8 +27294,11 @@
       <c r="AW169" s="50">
         <v>12</v>
       </c>
+      <c r="AX169" s="50">
+        <v>13</v>
+      </c>
     </row>
-    <row r="170" spans="1:49" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="170" spans="1:50" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A170" s="31" t="s">
         <v>168</v>
       </c>
@@ -26939,8 +27446,11 @@
       <c r="AW170" s="50">
         <v>0</v>
       </c>
+      <c r="AX170" s="50">
+        <v>0</v>
+      </c>
     </row>
-    <row r="171" spans="1:49" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="171" spans="1:50" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A171" s="26" t="s">
         <v>169</v>
       </c>
@@ -27088,8 +27598,11 @@
       <c r="AW171" s="50">
         <v>1</v>
       </c>
+      <c r="AX171" s="50">
+        <v>1</v>
+      </c>
     </row>
-    <row r="172" spans="1:49" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="172" spans="1:50" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A172" s="26" t="s">
         <v>170</v>
       </c>
@@ -27237,8 +27750,11 @@
       <c r="AW172" s="50">
         <v>6</v>
       </c>
+      <c r="AX172" s="50">
+        <v>6</v>
+      </c>
     </row>
-    <row r="173" spans="1:49" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="173" spans="1:50" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A173" s="26" t="s">
         <v>171</v>
       </c>
@@ -27386,8 +27902,11 @@
       <c r="AW173" s="50">
         <v>417</v>
       </c>
+      <c r="AX173" s="50">
+        <v>440</v>
+      </c>
     </row>
-    <row r="174" spans="1:49" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="174" spans="1:50" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A174" s="26" t="s">
         <v>172</v>
       </c>
@@ -27535,8 +28054,11 @@
       <c r="AW174" s="50">
         <v>162</v>
       </c>
+      <c r="AX174" s="50">
+        <v>172</v>
+      </c>
     </row>
-    <row r="175" spans="1:49" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="175" spans="1:50" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A175" s="26" t="s">
         <v>173</v>
       </c>
@@ -27684,8 +28206,11 @@
       <c r="AW175" s="50">
         <v>5</v>
       </c>
+      <c r="AX175" s="50">
+        <v>5</v>
+      </c>
     </row>
-    <row r="176" spans="1:49" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="176" spans="1:50" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A176" s="26" t="s">
         <v>174</v>
       </c>
@@ -27833,8 +28358,11 @@
       <c r="AW176" s="50">
         <v>1</v>
       </c>
+      <c r="AX176" s="50">
+        <v>1</v>
+      </c>
     </row>
-    <row r="177" spans="1:49" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="177" spans="1:50" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A177" s="26" t="s">
         <v>175</v>
       </c>
@@ -27982,8 +28510,11 @@
       <c r="AW177" s="50">
         <v>98</v>
       </c>
+      <c r="AX177" s="50">
+        <v>110</v>
+      </c>
     </row>
-    <row r="178" spans="1:49" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="178" spans="1:50" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A178" s="26" t="s">
         <v>176</v>
       </c>
@@ -28131,8 +28662,11 @@
       <c r="AW178" s="50">
         <v>24</v>
       </c>
+      <c r="AX178" s="50">
+        <v>25</v>
+      </c>
     </row>
-    <row r="179" spans="1:49" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="179" spans="1:50" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A179" s="26" t="s">
         <v>177</v>
       </c>
@@ -28280,8 +28814,11 @@
       <c r="AW179" s="50">
         <v>2</v>
       </c>
+      <c r="AX179" s="50">
+        <v>2</v>
+      </c>
     </row>
-    <row r="180" spans="1:49" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="180" spans="1:50" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A180" s="26" t="s">
         <v>178</v>
       </c>
@@ -28429,8 +28966,11 @@
       <c r="AW180" s="50">
         <v>0</v>
       </c>
+      <c r="AX180" s="50">
+        <v>0</v>
+      </c>
     </row>
-    <row r="181" spans="1:49" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="181" spans="1:50" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A181" s="26" t="s">
         <v>179</v>
       </c>
@@ -28578,8 +29118,11 @@
       <c r="AW181" s="50">
         <v>90</v>
       </c>
+      <c r="AX181" s="50">
+        <v>90</v>
+      </c>
     </row>
-    <row r="182" spans="1:49" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="182" spans="1:50" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A182" s="26" t="s">
         <v>180</v>
       </c>
@@ -28727,8 +29270,11 @@
       <c r="AW182" s="50">
         <v>0</v>
       </c>
+      <c r="AX182" s="50">
+        <v>0</v>
+      </c>
     </row>
-    <row r="183" spans="1:49" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="183" spans="1:50" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A183" s="26" t="s">
         <v>181</v>
       </c>
@@ -28876,8 +29422,11 @@
       <c r="AW183" s="50">
         <v>3</v>
       </c>
+      <c r="AX183" s="50">
+        <v>3</v>
+      </c>
     </row>
-    <row r="184" spans="1:49" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="184" spans="1:50" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A184" s="26" t="s">
         <v>182</v>
       </c>
@@ -29025,8 +29574,11 @@
       <c r="AW184" s="50">
         <v>59</v>
       </c>
+      <c r="AX184" s="50">
+        <v>59</v>
+      </c>
     </row>
-    <row r="185" spans="1:49" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="185" spans="1:50" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A185" s="26" t="s">
         <v>183</v>
       </c>
@@ -29174,8 +29726,11 @@
       <c r="AW185" s="50">
         <v>7</v>
       </c>
+      <c r="AX185" s="50">
+        <v>7</v>
+      </c>
     </row>
-    <row r="186" spans="1:49" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="186" spans="1:50" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A186" s="26" t="s">
         <v>184</v>
       </c>
@@ -29323,8 +29878,11 @@
       <c r="AW186" s="50">
         <v>49</v>
       </c>
+      <c r="AX186" s="50">
+        <v>61</v>
+      </c>
     </row>
-    <row r="187" spans="1:49" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="187" spans="1:50" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A187" s="26" t="s">
         <v>185</v>
       </c>
@@ -29472,8 +30030,11 @@
       <c r="AW187" s="50">
         <v>21</v>
       </c>
+      <c r="AX187" s="50">
+        <v>22</v>
+      </c>
     </row>
-    <row r="188" spans="1:49" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="188" spans="1:50" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A188" s="26" t="s">
         <v>186</v>
       </c>
@@ -29621,8 +30182,11 @@
       <c r="AW188" s="50">
         <v>3</v>
       </c>
+      <c r="AX188" s="50">
+        <v>3</v>
+      </c>
     </row>
-    <row r="189" spans="1:49" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="189" spans="1:50" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A189" s="26" t="s">
         <v>187</v>
       </c>
@@ -29770,8 +30334,11 @@
       <c r="AW189" s="50">
         <v>5</v>
       </c>
+      <c r="AX189" s="50">
+        <v>6</v>
+      </c>
     </row>
-    <row r="190" spans="1:49" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="190" spans="1:50" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A190" s="26" t="s">
         <v>188</v>
       </c>
@@ -29919,8 +30486,11 @@
       <c r="AW190" s="50">
         <v>15</v>
       </c>
+      <c r="AX190" s="50">
+        <v>17</v>
+      </c>
     </row>
-    <row r="191" spans="1:49" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="191" spans="1:50" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A191" s="26" t="s">
         <v>189</v>
       </c>
@@ -30068,8 +30638,11 @@
       <c r="AW191" s="50">
         <v>174</v>
       </c>
+      <c r="AX191" s="50">
+        <v>204</v>
+      </c>
     </row>
-    <row r="192" spans="1:49" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="192" spans="1:50" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A192" s="26" t="s">
         <v>190</v>
       </c>
@@ -30217,8 +30790,11 @@
       <c r="AW192" s="50">
         <v>0</v>
       </c>
+      <c r="AX192" s="50">
+        <v>0</v>
+      </c>
     </row>
-    <row r="193" spans="1:49" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="193" spans="1:50" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A193" s="26" t="s">
         <v>191</v>
       </c>
@@ -30366,8 +30942,11 @@
       <c r="AW193" s="50">
         <v>2</v>
       </c>
+      <c r="AX193" s="50">
+        <v>2</v>
+      </c>
     </row>
-    <row r="194" spans="1:49" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="194" spans="1:50" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A194" s="26" t="s">
         <v>192</v>
       </c>
@@ -30515,8 +31094,11 @@
       <c r="AW194" s="50">
         <v>117</v>
       </c>
+      <c r="AX194" s="50">
+        <v>125</v>
+      </c>
     </row>
-    <row r="195" spans="1:49" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="195" spans="1:50" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A195" s="26" t="s">
         <v>193</v>
       </c>
@@ -30664,8 +31246,11 @@
       <c r="AW195" s="50">
         <v>0</v>
       </c>
+      <c r="AX195" s="50">
+        <v>0</v>
+      </c>
     </row>
-    <row r="196" spans="1:49" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="196" spans="1:50" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A196" s="26" t="s">
         <v>194</v>
       </c>
@@ -30813,8 +31398,11 @@
       <c r="AW196" s="50">
         <v>0</v>
       </c>
+      <c r="AX196" s="50">
+        <v>0</v>
+      </c>
     </row>
-    <row r="197" spans="1:49" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="197" spans="1:50" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A197" s="26" t="s">
         <v>195</v>
       </c>
@@ -30962,8 +31550,11 @@
       <c r="AW197" s="50">
         <v>1</v>
       </c>
+      <c r="AX197" s="50">
+        <v>1</v>
+      </c>
     </row>
-    <row r="198" spans="1:49" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="198" spans="1:50" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A198" s="26" t="s">
         <v>196</v>
       </c>
@@ -31111,8 +31702,11 @@
       <c r="AW198" s="50">
         <v>0</v>
       </c>
+      <c r="AX198" s="50">
+        <v>0</v>
+      </c>
     </row>
-    <row r="199" spans="1:49" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="199" spans="1:50" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A199" s="26" t="s">
         <v>197</v>
       </c>
@@ -31260,8 +31854,11 @@
       <c r="AW199" s="50">
         <v>0</v>
       </c>
+      <c r="AX199" s="50">
+        <v>0</v>
+      </c>
     </row>
-    <row r="200" spans="1:49" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="200" spans="1:50" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A200" s="26" t="s">
         <v>198</v>
       </c>
@@ -31409,8 +32006,11 @@
       <c r="AW200" s="50">
         <v>2</v>
       </c>
+      <c r="AX200" s="50">
+        <v>2</v>
+      </c>
     </row>
-    <row r="201" spans="1:49" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="201" spans="1:50" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A201" s="26" t="s">
         <v>199</v>
       </c>
@@ -31558,8 +32158,11 @@
       <c r="AW201" s="50">
         <v>2</v>
       </c>
+      <c r="AX201" s="50">
+        <v>2</v>
+      </c>
     </row>
-    <row r="202" spans="1:49" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="202" spans="1:50" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A202" s="26" t="s">
         <v>200</v>
       </c>
@@ -31707,8 +32310,11 @@
       <c r="AW202" s="50">
         <v>48</v>
       </c>
+      <c r="AX202" s="50">
+        <v>48</v>
+      </c>
     </row>
-    <row r="203" spans="1:49" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="203" spans="1:50" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A203" s="26" t="s">
         <v>201</v>
       </c>
@@ -31856,8 +32462,11 @@
       <c r="AW203" s="50">
         <v>0</v>
       </c>
+      <c r="AX203" s="50">
+        <v>0</v>
+      </c>
     </row>
-    <row r="204" spans="1:49" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="204" spans="1:50" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A204" s="26" t="s">
         <v>202</v>
       </c>
@@ -32005,8 +32614,11 @@
       <c r="AW204" s="50">
         <v>28</v>
       </c>
+      <c r="AX204" s="50">
+        <v>28</v>
+      </c>
     </row>
-    <row r="205" spans="1:49" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="205" spans="1:50" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A205" s="26" t="s">
         <v>203</v>
       </c>
@@ -32154,8 +32766,11 @@
       <c r="AW205" s="50">
         <v>1</v>
       </c>
+      <c r="AX205" s="50">
+        <v>1</v>
+      </c>
     </row>
-    <row r="206" spans="1:49" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="206" spans="1:50" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A206" s="26" t="s">
         <v>204</v>
       </c>
@@ -32303,8 +32918,11 @@
       <c r="AW206" s="50">
         <v>14</v>
       </c>
+      <c r="AX206" s="50">
+        <v>15</v>
+      </c>
     </row>
-    <row r="207" spans="1:49" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="207" spans="1:50" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A207" s="26" t="s">
         <v>205</v>
       </c>
@@ -32452,8 +33070,11 @@
       <c r="AW207" s="50">
         <v>8</v>
       </c>
+      <c r="AX207" s="50">
+        <v>8</v>
+      </c>
     </row>
-    <row r="208" spans="1:49" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="208" spans="1:50" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A208" s="26" t="s">
         <v>206</v>
       </c>
@@ -32601,8 +33222,11 @@
       <c r="AW208" s="50">
         <v>9</v>
       </c>
+      <c r="AX208" s="50">
+        <v>11</v>
+      </c>
     </row>
-    <row r="209" spans="1:49" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="209" spans="1:50" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A209" s="26" t="s">
         <v>207</v>
       </c>
@@ -32750,8 +33374,11 @@
       <c r="AW209" s="50">
         <v>0</v>
       </c>
+      <c r="AX209" s="50">
+        <v>0</v>
+      </c>
     </row>
-    <row r="210" spans="1:49" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="210" spans="1:50" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A210" s="26" t="s">
         <v>208</v>
       </c>
@@ -32899,8 +33526,11 @@
       <c r="AW210" s="50">
         <v>0</v>
       </c>
+      <c r="AX210" s="50">
+        <v>0</v>
+      </c>
     </row>
-    <row r="211" spans="1:49" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="211" spans="1:50" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A211" s="26" t="s">
         <v>209</v>
       </c>
@@ -33048,8 +33678,11 @@
       <c r="AW211" s="50">
         <v>2</v>
       </c>
+      <c r="AX211" s="50">
+        <v>2</v>
+      </c>
     </row>
-    <row r="212" spans="1:49" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="212" spans="1:50" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A212" s="26" t="s">
         <v>210</v>
       </c>
@@ -33197,8 +33830,11 @@
       <c r="AW212" s="50">
         <v>0</v>
       </c>
+      <c r="AX212" s="50">
+        <v>0</v>
+      </c>
     </row>
-    <row r="213" spans="1:49" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="213" spans="1:50" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A213" s="26" t="s">
         <v>211</v>
       </c>
@@ -33346,8 +33982,11 @@
       <c r="AW213" s="50">
         <v>69</v>
       </c>
+      <c r="AX213" s="50">
+        <v>85</v>
+      </c>
     </row>
-    <row r="214" spans="1:49" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="214" spans="1:50" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A214" s="26" t="s">
         <v>212</v>
       </c>
@@ -33495,8 +34134,11 @@
       <c r="AW214" s="50">
         <v>9</v>
       </c>
+      <c r="AX214" s="50">
+        <v>10</v>
+      </c>
     </row>
-    <row r="215" spans="1:49" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="215" spans="1:50" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A215" s="26" t="s">
         <v>213</v>
       </c>
@@ -33644,8 +34286,11 @@
       <c r="AW215" s="50">
         <v>124</v>
       </c>
+      <c r="AX215" s="50">
+        <v>125</v>
+      </c>
     </row>
-    <row r="216" spans="1:49" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="216" spans="1:50" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A216" s="26" t="s">
         <v>214</v>
       </c>
@@ -33793,8 +34438,11 @@
       <c r="AW216" s="50">
         <v>0</v>
       </c>
+      <c r="AX216" s="50">
+        <v>0</v>
+      </c>
     </row>
-    <row r="217" spans="1:49" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="217" spans="1:50" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A217" s="26" t="s">
         <v>215</v>
       </c>
@@ -33942,8 +34590,11 @@
       <c r="AW217" s="50">
         <v>7</v>
       </c>
+      <c r="AX217" s="50">
+        <v>7</v>
+      </c>
     </row>
-    <row r="218" spans="1:49" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="218" spans="1:50" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A218" s="26" t="s">
         <v>216</v>
       </c>
@@ -34091,8 +34742,11 @@
       <c r="AW218" s="50">
         <v>1</v>
       </c>
+      <c r="AX218" s="50">
+        <v>1</v>
+      </c>
     </row>
-    <row r="219" spans="1:49" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="219" spans="1:50" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A219" s="26" t="s">
         <v>217</v>
       </c>
@@ -34240,8 +34894,11 @@
       <c r="AW219" s="50">
         <v>0</v>
       </c>
+      <c r="AX219" s="50">
+        <v>0</v>
+      </c>
     </row>
-    <row r="220" spans="1:49" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="220" spans="1:50" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A220" s="26" t="s">
         <v>218</v>
       </c>
@@ -34389,8 +35046,11 @@
       <c r="AW220" s="50">
         <v>0</v>
       </c>
+      <c r="AX220" s="50">
+        <v>0</v>
+      </c>
     </row>
-    <row r="221" spans="1:49" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="221" spans="1:50" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A221" s="26" t="s">
         <v>219</v>
       </c>
@@ -34538,8 +35198,11 @@
       <c r="AW221" s="50">
         <v>0</v>
       </c>
+      <c r="AX221" s="50">
+        <v>0</v>
+      </c>
     </row>
-    <row r="222" spans="1:49" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="222" spans="1:50" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A222" s="26" t="s">
         <v>220</v>
       </c>
@@ -34687,8 +35350,11 @@
       <c r="AW222" s="50">
         <v>6</v>
       </c>
+      <c r="AX222" s="50">
+        <v>6</v>
+      </c>
     </row>
-    <row r="223" spans="1:49" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="223" spans="1:50" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A223" s="26" t="s">
         <v>221</v>
       </c>
@@ -34836,8 +35502,11 @@
       <c r="AW223" s="50">
         <v>1333</v>
       </c>
+      <c r="AX223" s="50">
+        <v>1430</v>
+      </c>
     </row>
-    <row r="224" spans="1:49" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="224" spans="1:50" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A224" s="26" t="s">
         <v>222</v>
       </c>
@@ -34985,8 +35654,11 @@
       <c r="AW224" s="50">
         <v>164</v>
       </c>
+      <c r="AX224" s="50">
+        <v>185</v>
+      </c>
     </row>
-    <row r="225" spans="1:49" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="225" spans="1:50" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A225" s="26" t="s">
         <v>223</v>
       </c>
@@ -35134,8 +35806,11 @@
       <c r="AW225" s="50">
         <v>0</v>
       </c>
+      <c r="AX225" s="50">
+        <v>0</v>
+      </c>
     </row>
-    <row r="226" spans="1:49" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="226" spans="1:50" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A226" s="26" t="s">
         <v>224</v>
       </c>
@@ -35283,8 +35958,11 @@
       <c r="AW226" s="50">
         <v>10</v>
       </c>
+      <c r="AX226" s="50">
+        <v>10</v>
+      </c>
     </row>
-    <row r="227" spans="1:49" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="227" spans="1:50" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A227" s="26" t="s">
         <v>225</v>
       </c>
@@ -35432,8 +36110,11 @@
       <c r="AW227" s="50">
         <v>0</v>
       </c>
+      <c r="AX227" s="50">
+        <v>0</v>
+      </c>
     </row>
-    <row r="228" spans="1:49" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="228" spans="1:50" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A228" s="26" t="s">
         <v>226</v>
       </c>
@@ -35581,8 +36262,11 @@
       <c r="AW228" s="50">
         <v>12</v>
       </c>
+      <c r="AX228" s="50">
+        <v>12</v>
+      </c>
     </row>
-    <row r="229" spans="1:49" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="229" spans="1:50" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A229" s="26" t="s">
         <v>227</v>
       </c>
@@ -35730,8 +36414,11 @@
       <c r="AW229" s="50">
         <v>41</v>
       </c>
+      <c r="AX229" s="50">
+        <v>41</v>
+      </c>
     </row>
-    <row r="230" spans="1:49" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="230" spans="1:50" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A230" s="26" t="s">
         <v>228</v>
       </c>
@@ -35879,8 +36566,11 @@
       <c r="AW230" s="50">
         <v>1233</v>
       </c>
+      <c r="AX230" s="50">
+        <v>1263</v>
+      </c>
     </row>
-    <row r="231" spans="1:49" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="231" spans="1:50" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A231" s="26" t="s">
         <v>229</v>
       </c>
@@ -36028,8 +36718,11 @@
       <c r="AW231" s="50">
         <v>7</v>
       </c>
+      <c r="AX231" s="50">
+        <v>7</v>
+      </c>
     </row>
-    <row r="232" spans="1:49" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="232" spans="1:50" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A232" s="26" t="s">
         <v>230</v>
       </c>
@@ -36177,8 +36870,11 @@
       <c r="AW232" s="50">
         <v>6</v>
       </c>
+      <c r="AX232" s="50">
+        <v>6</v>
+      </c>
     </row>
-    <row r="233" spans="1:49" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="233" spans="1:50" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A233" s="26" t="s">
         <v>231</v>
       </c>
@@ -36326,8 +37022,11 @@
       <c r="AW233" s="50">
         <v>12</v>
       </c>
+      <c r="AX233" s="50">
+        <v>12</v>
+      </c>
     </row>
-    <row r="234" spans="1:49" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="234" spans="1:50" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A234" s="26" t="s">
         <v>232</v>
       </c>
@@ -36475,8 +37174,11 @@
       <c r="AW234" s="50">
         <v>0</v>
       </c>
+      <c r="AX234" s="50">
+        <v>0</v>
+      </c>
     </row>
-    <row r="235" spans="1:49" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="235" spans="1:50" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A235" s="26" t="s">
         <v>233</v>
       </c>
@@ -36624,8 +37326,11 @@
       <c r="AW235" s="50">
         <v>6</v>
       </c>
+      <c r="AX235" s="50">
+        <v>6</v>
+      </c>
     </row>
-    <row r="236" spans="1:49" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="236" spans="1:50" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A236" s="26" t="s">
         <v>234</v>
       </c>
@@ -36773,8 +37478,11 @@
       <c r="AW236" s="50">
         <v>12</v>
       </c>
+      <c r="AX236" s="50">
+        <v>12</v>
+      </c>
     </row>
-    <row r="237" spans="1:49" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="237" spans="1:50" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A237" s="26" t="s">
         <v>235</v>
       </c>
@@ -36922,8 +37630,11 @@
       <c r="AW237" s="50">
         <v>13</v>
       </c>
+      <c r="AX237" s="50">
+        <v>13</v>
+      </c>
     </row>
-    <row r="238" spans="1:49" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="238" spans="1:50" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A238" s="26" t="s">
         <v>236</v>
       </c>
@@ -37071,8 +37782,11 @@
       <c r="AW238" s="50">
         <v>96</v>
       </c>
+      <c r="AX238" s="50">
+        <v>105</v>
+      </c>
     </row>
-    <row r="239" spans="1:49" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="239" spans="1:50" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A239" s="26" t="s">
         <v>237</v>
       </c>
@@ -37220,8 +37934,11 @@
       <c r="AW239" s="50">
         <v>95</v>
       </c>
+      <c r="AX239" s="50">
+        <v>136</v>
+      </c>
     </row>
-    <row r="240" spans="1:49" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="240" spans="1:50" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A240" s="26" t="s">
         <v>238</v>
       </c>
@@ -37369,8 +38086,11 @@
       <c r="AW240" s="50">
         <v>27</v>
       </c>
+      <c r="AX240" s="50">
+        <v>25</v>
+      </c>
     </row>
-    <row r="241" spans="1:49" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="241" spans="1:50" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A241" s="26" t="s">
         <v>239</v>
       </c>
@@ -37518,8 +38238,11 @@
       <c r="AW241" s="50">
         <v>0</v>
       </c>
+      <c r="AX241" s="50">
+        <v>0</v>
+      </c>
     </row>
-    <row r="242" spans="1:49" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="242" spans="1:50" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A242" s="26" t="s">
         <v>240</v>
       </c>
@@ -37667,8 +38390,11 @@
       <c r="AW242" s="50">
         <v>71</v>
       </c>
+      <c r="AX242" s="50">
+        <v>77</v>
+      </c>
     </row>
-    <row r="243" spans="1:49" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="243" spans="1:50" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A243" s="26" t="s">
         <v>241</v>
       </c>
@@ -37816,8 +38542,11 @@
       <c r="AW243" s="50">
         <v>295</v>
       </c>
+      <c r="AX243" s="50">
+        <v>302</v>
+      </c>
     </row>
-    <row r="244" spans="1:49" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="244" spans="1:50" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A244" s="26" t="s">
         <v>242</v>
       </c>
@@ -37965,8 +38694,11 @@
       <c r="AW244" s="50">
         <v>36</v>
       </c>
+      <c r="AX244" s="50">
+        <v>36</v>
+      </c>
     </row>
-    <row r="245" spans="1:49" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="245" spans="1:50" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A245" s="26" t="s">
         <v>243</v>
       </c>
@@ -38114,8 +38846,11 @@
       <c r="AW245" s="50">
         <v>1</v>
       </c>
+      <c r="AX245" s="50">
+        <v>1</v>
+      </c>
     </row>
-    <row r="246" spans="1:49" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="246" spans="1:50" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A246" s="26" t="s">
         <v>244</v>
       </c>
@@ -38263,8 +38998,11 @@
       <c r="AW246" s="50">
         <v>62</v>
       </c>
+      <c r="AX246" s="50">
+        <v>62</v>
+      </c>
     </row>
-    <row r="247" spans="1:49" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="247" spans="1:50" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A247" s="26" t="s">
         <v>245</v>
       </c>
@@ -38412,8 +39150,11 @@
       <c r="AW247" s="50">
         <v>1</v>
       </c>
+      <c r="AX247" s="50">
+        <v>1</v>
+      </c>
     </row>
-    <row r="248" spans="1:49" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="248" spans="1:50" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A248" s="26" t="s">
         <v>246</v>
       </c>
@@ -38561,8 +39302,11 @@
       <c r="AW248" s="50">
         <v>10</v>
       </c>
+      <c r="AX248" s="50">
+        <v>10</v>
+      </c>
     </row>
-    <row r="249" spans="1:49" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="249" spans="1:50" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A249" s="26" t="s">
         <v>247</v>
       </c>
@@ -38710,8 +39454,11 @@
       <c r="AW249" s="50">
         <v>158</v>
       </c>
+      <c r="AX249" s="50">
+        <v>167</v>
+      </c>
     </row>
-    <row r="250" spans="1:49" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="250" spans="1:50" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A250" s="26" t="s">
         <v>248</v>
       </c>
@@ -38859,8 +39606,11 @@
       <c r="AW250" s="50">
         <v>23</v>
       </c>
+      <c r="AX250" s="50">
+        <v>25</v>
+      </c>
     </row>
-    <row r="251" spans="1:49" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="251" spans="1:50" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A251" s="26" t="s">
         <v>249</v>
       </c>
@@ -39008,8 +39758,11 @@
       <c r="AW251" s="50">
         <v>3</v>
       </c>
+      <c r="AX251" s="50">
+        <v>3</v>
+      </c>
     </row>
-    <row r="252" spans="1:49" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="252" spans="1:50" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A252" s="26" t="s">
         <v>250</v>
       </c>
@@ -39157,8 +39910,11 @@
       <c r="AW252" s="50">
         <v>13</v>
       </c>
+      <c r="AX252" s="50">
+        <v>14</v>
+      </c>
     </row>
-    <row r="253" spans="1:49" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="253" spans="1:50" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A253" s="26" t="s">
         <v>251</v>
       </c>
@@ -39306,8 +40062,11 @@
       <c r="AW253" s="50">
         <v>6</v>
       </c>
+      <c r="AX253" s="50">
+        <v>6</v>
+      </c>
     </row>
-    <row r="254" spans="1:49" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="254" spans="1:50" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A254" s="26" t="s">
         <v>252</v>
       </c>
@@ -39455,8 +40214,11 @@
       <c r="AW254" s="50">
         <v>1</v>
       </c>
+      <c r="AX254" s="50">
+        <v>1</v>
+      </c>
     </row>
-    <row r="255" spans="1:49" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="255" spans="1:50" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A255" s="26" t="s">
         <v>253</v>
       </c>
@@ -39604,8 +40366,11 @@
       <c r="AW255" s="50">
         <v>4</v>
       </c>
+      <c r="AX255" s="50">
+        <v>4</v>
+      </c>
     </row>
-    <row r="256" spans="1:49" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="256" spans="1:50" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A256" s="26" t="s">
         <v>254</v>
       </c>
@@ -39753,8 +40518,11 @@
       <c r="AW256" s="50">
         <v>7</v>
       </c>
+      <c r="AX256" s="50">
+        <v>7</v>
+      </c>
     </row>
-    <row r="257" spans="1:49" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="257" spans="1:50" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A257" s="26" t="s">
         <v>255</v>
       </c>
@@ -39902,8 +40670,11 @@
       <c r="AW257" s="50">
         <v>1</v>
       </c>
+      <c r="AX257" s="50">
+        <v>1</v>
+      </c>
     </row>
-    <row r="258" spans="1:49" ht="22.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="258" spans="1:50" ht="22.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A258" s="32" t="s">
         <v>1</v>
       </c>
@@ -40090,8 +40861,12 @@
         <f>SUM(AW4:AW257)</f>
         <v>21069</v>
       </c>
+      <c r="AX258" s="8">
+        <f>SUM(AX4:AX257)</f>
+        <v>21944</v>
+      </c>
     </row>
-    <row r="259" spans="1:49" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="259" spans="1:50" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="AI259" s="46"/>
       <c r="AJ259" s="46"/>
       <c r="AK259" s="46"/>
@@ -40107,8 +40882,9 @@
       <c r="AU259" s="51"/>
       <c r="AV259" s="51"/>
       <c r="AW259" s="51"/>
+      <c r="AX259" s="51"/>
     </row>
-    <row r="260" spans="1:49" s="35" customFormat="1" ht="31.15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="260" spans="1:50" s="35" customFormat="1" ht="31.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A260" s="33" t="s">
         <v>260</v>
       </c>
@@ -40298,12 +41074,16 @@
         <v>198</v>
       </c>
       <c r="AW260" s="52">
-        <f t="shared" ref="AW260" si="3">COUNTIF(AW4:AW257,"&lt;&gt;0")</f>
+        <f t="shared" ref="AW260:AX260" si="3">COUNTIF(AW4:AW257,"&lt;&gt;0")</f>
         <v>200</v>
       </c>
+      <c r="AX260" s="52">
+        <f t="shared" si="3"/>
+        <v>202</v>
+      </c>
     </row>
-    <row r="261" spans="1:49" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="262" spans="1:49" s="16" customFormat="1" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="261" spans="1:50" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="262" spans="1:50" s="16" customFormat="1" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A262" s="36" t="s">
         <v>258</v>
       </c>
@@ -40339,8 +41119,9 @@
       <c r="AU262" s="54"/>
       <c r="AV262" s="54"/>
       <c r="AW262" s="54"/>
+      <c r="AX262" s="54"/>
     </row>
-    <row r="263" spans="1:49" s="16" customFormat="1" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="263" spans="1:50" s="16" customFormat="1" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A263" s="38" t="s">
         <v>287</v>
       </c>
@@ -40379,8 +41160,9 @@
       <c r="AU263" s="54"/>
       <c r="AV263" s="54"/>
       <c r="AW263" s="54"/>
+      <c r="AX263" s="54"/>
     </row>
-    <row r="264" spans="1:49" s="18" customFormat="1" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="264" spans="1:50" s="18" customFormat="1" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A264" s="39" t="s">
         <v>290</v>
       </c>
@@ -40408,8 +41190,9 @@
       <c r="AU264" s="55"/>
       <c r="AV264" s="55"/>
       <c r="AW264" s="55"/>
+      <c r="AX264" s="55"/>
     </row>
-    <row r="265" spans="1:49" s="16" customFormat="1" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="265" spans="1:50" s="16" customFormat="1" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A265" s="40" t="s">
         <v>281</v>
       </c>
@@ -40446,8 +41229,9 @@
       <c r="AU265" s="54"/>
       <c r="AV265" s="54"/>
       <c r="AW265" s="54"/>
+      <c r="AX265" s="54"/>
     </row>
-    <row r="266" spans="1:49" s="16" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="266" spans="1:50" s="16" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A266" s="36" t="s">
         <v>283</v>
       </c>
@@ -40484,8 +41268,9 @@
       <c r="AU266" s="54"/>
       <c r="AV266" s="54"/>
       <c r="AW266" s="54"/>
+      <c r="AX266" s="54"/>
     </row>
-    <row r="267" spans="1:49" s="16" customFormat="1" ht="50.65" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="267" spans="1:50" s="16" customFormat="1" ht="50.65" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A267" s="56" t="s">
         <v>289</v>
       </c>
@@ -40521,16 +41306,17 @@
       <c r="AU267" s="54"/>
       <c r="AV267" s="54"/>
       <c r="AW267" s="54"/>
+      <c r="AX267" s="54"/>
     </row>
-    <row r="268" spans="1:49" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="269" spans="1:49" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="268" spans="1:50" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="269" spans="1:50" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A269" s="11" t="s">
         <v>274</v>
       </c>
     </row>
-    <row r="270" spans="1:49" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="271" spans="1:49" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="272" spans="1:49" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="270" spans="1:50" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="271" spans="1:50" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="272" spans="1:50" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="273" spans="1:1" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A273" s="11" t="s">
         <v>274</v>

</xml_diff>